<commit_message>
Changes in helpFiles add programs in demo
</commit_message>
<xml_diff>
--- a/Tutorials_helpFiles/Core_Java_Brushup.xlsx
+++ b/Tutorials_helpFiles/Core_Java_Brushup.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alogaur\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rahul\Advance_topic\Tutorials_helpFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D24DBB1-1AF5-4951-A641-104A593BDB1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{45FE8B6A-A6B7-4791-857A-3D25D5E2D67B}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Overall " sheetId="1" r:id="rId1"/>
     <sheet name="Must Prepare" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>     Generics, wild card characters.</t>
   </si>
@@ -58,9 +57,6 @@
     <t>       How TreeSet works ?</t>
   </si>
   <si>
-    <t>      How to count internal iterations of lambda expression.</t>
-  </si>
-  <si>
     <t>       What is functional programming and structural programming.</t>
   </si>
   <si>
@@ -254,12 +250,15 @@
   </si>
   <si>
     <t>15. Difference between component and service annotations. </t>
+  </si>
+  <si>
+    <t>      How to count internal iterations of lambda expression. --&gt;  count =(int) list.stream().peek(x-&gt;System.out.println(x)).count();</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,18 +367,46 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -687,30 +714,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A68187A-1B79-4950-91D7-1E627D962722}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="2" width="159.36328125" customWidth="1"/>
-    <col min="3" max="3" width="45.36328125" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="2"/>
+    <col min="2" max="2" width="159.42578125" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -718,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -726,7 +753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -734,7 +761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -742,7 +769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -750,7 +777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -759,7 +786,7 @@
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -767,7 +794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -775,349 +802,349 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="6" t="s">
+      <c r="B37" s="4"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="4"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="4"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="4"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="4"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="4"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="4"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="4"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="4"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="4"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="4"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="4"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="4"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="4"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="4"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="4"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="4"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="4"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="4"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="4"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="4"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="4"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="4"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="4"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="4"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="4"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="4"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" s="4"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" s="4"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" s="4"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="4"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" s="4"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53" s="4"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B54" s="4"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B55" s="4"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" s="4"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" s="4"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="B58" s="4"/>
     </row>
@@ -1131,91 +1158,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C3508DA-2A45-4132-A8BF-6E6363A63B1C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="87.6328125" customWidth="1"/>
+    <col min="2" max="2" width="87.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B3" s="7" t="s">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B4" s="7" t="s">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B5" s="7" t="s">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B6" s="7" t="s">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B7" s="7" t="s">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B8" s="7" t="s">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B9" s="7" t="s">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B10" s="7" t="s">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B11" s="7" t="s">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B12" s="7" t="s">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B13" s="7" t="s">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B14" s="7" t="s">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B15" s="7" t="s">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B16" s="7" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>